<commit_message>
Módulo 05 - condicionais e operadores lógicos
</commit_message>
<xml_diff>
--- a/módulo 05/aula-formulas-logica.xlsx
+++ b/módulo 05/aula-formulas-logica.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Google Drive\Curso_Excel\05 Primeiras fórmulas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B898D61E-7C34-4D44-B9F0-365F00D2B175}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{9677FD8D-6660-41E5-9A81-FFEA2AD51EE9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="8" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Cad_Veículos" sheetId="10" r:id="rId3"/>
     <sheet name="Cad_Motorista" sheetId="11" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>EMPRESA</t>
   </si>
@@ -176,11 +175,29 @@
   <si>
     <t>Teste</t>
   </si>
+  <si>
+    <t xml:space="preserve">operadores lógicos: </t>
+  </si>
+  <si>
+    <t>&lt;&gt; : diferente</t>
+  </si>
+  <si>
+    <t>&gt; maior</t>
+  </si>
+  <si>
+    <t>&lt;menor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = igual</t>
+  </si>
+  <si>
+    <t>Se</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="\(##\)\ 0\ 0000&quot;-&quot;0000"/>
@@ -327,7 +344,194 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -361,7 +565,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6BA0FC6-3102-4105-B76E-A3425C0258A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -444,7 +648,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{29F412B0-641D-4F8B-B908-24115BAD6C2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -564,7 +768,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DCF631DB-37CE-486B-B435-8473605BF212}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -645,7 +849,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C08429E-7AEF-47DA-9312-B3EFFFD47D63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -726,7 +930,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EEB3F770-62EA-44CF-A1B6-CBDB1F0154E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -804,7 +1008,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2899AFD7-F534-4291-A4B0-8AAF42D3C45B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -888,7 +1092,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3627734-0663-4FA9-8780-F55E760F1049}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -969,7 +1173,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FC11C314-5AC1-4502-847C-2E61C5CAC00B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1089,7 +1293,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A018AF23-8EA1-4733-ADD0-8BD8E14326F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1172,7 +1376,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B68638E9-237B-4AB4-BD76-E5FF66A2646F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1253,7 +1457,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{78A4E03F-FBDB-42CE-9CEF-F8500D7571E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1535,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8C2157E-B594-4473-AB0A-20088837B6C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1614,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0024708-7F6B-4F06-A977-802C798E7611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1492,7 +1696,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F871882-370C-4E6B-9ED5-6934223D9A2A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1580,7 +1784,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A64CEA9A-4C88-4133-9DF5-BE5DB64BED22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1673,7 +1877,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F2EF660-7474-4CD1-B077-0422EA1DE591}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1754,7 +1958,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16FDE091-B1C0-4486-BEC7-834E97580F0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1874,7 +2078,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C29C9295-0E79-43A4-A139-C0D744B4C204}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1957,7 +2161,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7C5A30B4-9A56-48C5-A173-5F0E10A7AB7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2038,7 +2242,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D12ED82-1966-40CD-9E3C-05EF439074E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2116,7 +2320,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3E0851EE-3980-4CF3-9523-FD6F20A09F57}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2195,7 +2399,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00BE3D7A-4446-4BEA-A7CB-DB25B6586066}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2283,7 +2487,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CB659196-ECF7-4D92-8830-DC4A35CF8B23}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2365,7 +2569,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1765B02A-B454-4EB9-8653-55C085C8D0BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2458,7 +2662,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{687357EC-8C7C-41E6-BC98-40CF0DB7E1CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2539,7 +2743,7 @@
         <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E273CD41-0863-4D4B-AD5E-C2F31D84A70C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2659,7 +2863,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DE7789A-574B-4EF5-AC20-13EE21124EE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2742,7 +2946,7 @@
         <xdr:cNvPr id="5" name="Retângulo: Cantos Superiores Recortados 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B93ABDEB-7E13-4C91-95D9-9FB5F6B1CC79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2823,7 +3027,7 @@
         <xdr:cNvPr id="6" name="Retângulo: Cantos Superiores Recortados 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB22967A-FF0E-4073-8C69-74EF7F36C182}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2901,7 +3105,7 @@
         <xdr:cNvPr id="7" name="Retângulo: Cantos Superiores Recortados 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{875BB76A-28F7-4C24-9428-5CF75AB39CDC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2980,7 +3184,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AA0C125-7FA2-42DD-A022-E130DCF31A2C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3068,7 +3272,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8ED9A2C-2351-485B-BE55-EACC611E479D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3156,7 +3360,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3EC9340D-B862-4EFA-A6D8-EE3E27D0E02F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3518,11 +3722,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46F83BD-F3BF-43E4-9A28-8E259EC6705F}">
-  <dimension ref="A1:P25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3598,14 +3802,84 @@
         <f>CONCATENATE(PROPER(Cad_Empresa!B14),", ",Cad_Empresa!B18," - ",PROPER(Cad_Empresa!B22))</f>
         <v>Rua Do Educador, 2500 - Uberlândia</v>
       </c>
-    </row>
-    <row r="25" spans="13:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="1">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1" t="b">
+        <f>E16&gt;F16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="b">
+        <f>E16&lt;F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="b">
+        <f>E16=F16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="b">
+        <f>E16&lt;&gt;F16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <f>AND(E16&gt;F16,E16&lt;&gt;F16)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="str">
+        <f>IF(E16&lt;0,"Negativo", IF(E16&gt;0, "Positivo","Nulo"))</f>
+        <v>Positivo</v>
+      </c>
+      <c r="D25" s="1" t="b">
+        <f>AND(E16&gt;F16,E16&lt;0)</f>
+        <v>0</v>
+      </c>
       <c r="M25" s="24">
         <f ca="1">TODAY()</f>
-        <v>43410</v>
+        <v>45350</v>
       </c>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="b">
+        <f>OR(E16&gt;F16,E16&lt;0)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3618,7 +3892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F21D338-352F-44D6-9932-736A440D777F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -3737,11 +4011,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596A196C-9CE3-40B9-AE7D-0ADEF9C03F4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3854,13 +4128,16 @@
       </c>
       <c r="I5" s="16">
         <f ca="1">(TODAY()-G5)/365</f>
-        <v>5.0712328767123287</v>
+        <v>10.386301369863014</v>
       </c>
       <c r="J5" s="17">
         <f>YEAR(G5)+5</f>
         <v>2018</v>
       </c>
-      <c r="K5" s="23"/>
+      <c r="K5" s="23" t="str">
+        <f ca="1">IF(I5&gt;=5,"Alta","Baixa")</f>
+        <v>Alta</v>
+      </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
@@ -3893,13 +4170,16 @@
       </c>
       <c r="I6" s="16">
         <f ca="1">(TODAY()-G6)/365</f>
-        <v>1.4438356164383561</v>
+        <v>6.7589041095890412</v>
       </c>
       <c r="J6" s="17">
         <f>YEAR(G6)+5</f>
         <v>2022</v>
       </c>
-      <c r="K6" s="23"/>
+      <c r="K6" s="23" t="str">
+        <f ca="1">IF(I6&gt;=5,"Alta","Baixa")</f>
+        <v>Alta</v>
+      </c>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -3914,11 +4194,19 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="15">
+        <v>44938</v>
+      </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="16"/>
+      <c r="I7" s="16">
+        <f ca="1">(TODAY()-G7)/365</f>
+        <v>1.1287671232876713</v>
+      </c>
       <c r="J7" s="17"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="23" t="str">
+        <f ca="1">IF(I7&gt;=5,"Alta","Baixa")</f>
+        <v>Baixa</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -4509,10 +4797,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tipo de combustível inválido!" error="Selecione um dos tipos de combustível disponíveis." sqref="E5:E31" xr:uid="{EBF39E31-3EFF-452C-8162-8407A658C179}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Tipo de combustível inválido!" error="Selecione um dos tipos de combustível disponíveis." sqref="E5:E31">
       <formula1>"Diesel,Etanol,Flex,Gasolina,GNV"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estado da compra inválido!" error="Selecione um dos tipos de estados da compra válidos." sqref="H5:H31" xr:uid="{FD2C5DED-2D25-49F7-871E-3ADDF2ABFECC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Estado da compra inválido!" error="Selecione um dos tipos de estados da compra válidos." sqref="H5:H31">
       <formula1>"Novo,Usado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4523,11 +4811,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E42239-30B6-4778-8F0C-BF94D02189A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4623,9 +4911,12 @@
         <v>34</v>
       </c>
       <c r="G5" s="15">
-        <v>43741</v>
-      </c>
-      <c r="H5" s="22"/>
+        <v>45568</v>
+      </c>
+      <c r="H5" s="22" t="str">
+        <f ca="1">IF(G5&gt;=TODAY(),"Em dia","Vencida")</f>
+        <v>Em dia</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -4656,7 +4947,10 @@
       <c r="G6" s="15">
         <v>43368</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="22" t="str">
+        <f t="shared" ref="H6:H8" ca="1" si="0">IF(G6&gt;=TODAY(),"Em dia","Vencida")</f>
+        <v>Vencida</v>
+      </c>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -4685,7 +4979,10 @@
       <c r="G7" s="15">
         <v>43439</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="22" t="str">
+        <f ca="1">IF(G7&gt;=TODAY(),"Em dia","Vencida")</f>
+        <v>Vencida</v>
+      </c>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -4705,8 +5002,11 @@
       <c r="D8" s="20"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="22" t="str">
+        <f ca="1">IF(G8=""," -- ", IF(G8&gt;=TODAY(),"Em dia","Vencida"))</f>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -4725,7 +5025,10 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="22"/>
+      <c r="H9" s="22" t="str">
+        <f t="shared" ref="H9:H16" ca="1" si="1">IF(G9=""," -- ", IF(G9&gt;=TODAY(),"Em dia","Vencida"))</f>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -4744,7 +5047,10 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -4761,7 +5067,10 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="22"/>
+      <c r="H11" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -4778,7 +5087,10 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="22"/>
+      <c r="H12" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -4795,7 +5107,10 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -4812,7 +5127,10 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -4829,7 +5147,10 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="15"/>
+      <c r="H15" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
@@ -4846,7 +5167,10 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v xml:space="preserve"> -- </v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -5422,8 +5746,18 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
+  <conditionalFormatting sqref="H5:H16">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="vencida">
+      <formula>NOT(ISERROR(SEARCH("vencida",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H16">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="Em dia">
+      <formula>NOT(ISERROR(SEARCH("Em dia",H5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Categoria Inválida!" error="Selecione uma das categorias disponíveis." sqref="F5:F18" xr:uid="{3E89EE8C-0A27-417A-B914-72104152AA8F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Categoria Inválida!" error="Selecione uma das categorias disponíveis." sqref="F5:F18">
       <formula1>"A,B,C,D,E,AB,AC,AD,AE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>